<commit_message>
updated occupation classifier (all states)
</commit_message>
<xml_diff>
--- a/S2022/comparison_between_debt_holders/avg_debt_occupation/FinishedSpreadsheets/OccupationsPA.xlsx
+++ b/S2022/comparison_between_debt_holders/avg_debt_occupation/FinishedSpreadsheets/OccupationsPA.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>occupation</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>inn keeper</t>
-  </si>
-  <si>
-    <t>junior</t>
   </si>
   <si>
     <t>marchant</t>
@@ -500,7 +497,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -566,7 +563,7 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>64008.84</v>
+        <v>74699.95999999999</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -753,7 +750,7 @@
         <v>23</v>
       </c>
       <c r="C23">
-        <v>10691.12</v>
+        <v>612574.61</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -764,7 +761,7 @@
         <v>24</v>
       </c>
       <c r="C24">
-        <v>612574.61</v>
+        <v>3906.5714</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -775,7 +772,7 @@
         <v>25</v>
       </c>
       <c r="C25">
-        <v>3906.5714</v>
+        <v>856.5599999999999</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -786,7 +783,7 @@
         <v>26</v>
       </c>
       <c r="C26">
-        <v>856.5599999999999</v>
+        <v>1769.01</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -797,7 +794,7 @@
         <v>27</v>
       </c>
       <c r="C27">
-        <v>1769.01</v>
+        <v>7083.53</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -808,7 +805,7 @@
         <v>28</v>
       </c>
       <c r="C28">
-        <v>7083.53</v>
+        <v>7717.74</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -819,7 +816,7 @@
         <v>29</v>
       </c>
       <c r="C29">
-        <v>7717.74</v>
+        <v>461.11</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -830,7 +827,7 @@
         <v>30</v>
       </c>
       <c r="C30">
-        <v>461.11</v>
+        <v>224.12</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -841,7 +838,7 @@
         <v>31</v>
       </c>
       <c r="C31">
-        <v>224.12</v>
+        <v>56.21</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -852,7 +849,7 @@
         <v>32</v>
       </c>
       <c r="C32">
-        <v>56.21</v>
+        <v>1241.76</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -863,7 +860,7 @@
         <v>33</v>
       </c>
       <c r="C33">
-        <v>1241.76</v>
+        <v>588.95</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -874,7 +871,7 @@
         <v>34</v>
       </c>
       <c r="C34">
-        <v>588.95</v>
+        <v>1917.65</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -885,7 +882,7 @@
         <v>35</v>
       </c>
       <c r="C35">
-        <v>1917.65</v>
+        <v>528.33</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -896,7 +893,7 @@
         <v>36</v>
       </c>
       <c r="C36">
-        <v>528.33</v>
+        <v>1192.25</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -907,7 +904,7 @@
         <v>37</v>
       </c>
       <c r="C37">
-        <v>1192.25</v>
+        <v>2137.39</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -918,7 +915,7 @@
         <v>38</v>
       </c>
       <c r="C38">
-        <v>2137.39</v>
+        <v>714.8099999999999</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -929,7 +926,7 @@
         <v>39</v>
       </c>
       <c r="C39">
-        <v>714.8099999999999</v>
+        <v>2054.64</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -940,7 +937,7 @@
         <v>40</v>
       </c>
       <c r="C40">
-        <v>2054.64</v>
+        <v>5576.53</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -951,17 +948,6 @@
         <v>41</v>
       </c>
       <c r="C41">
-        <v>5576.53</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="1">
-        <v>40</v>
-      </c>
-      <c r="B42" t="s">
-        <v>42</v>
-      </c>
-      <c r="C42">
         <v>1136.06</v>
       </c>
     </row>

</xml_diff>